<commit_message>
Updating stim gen files for tones to match dropbox
</commit_message>
<xml_diff>
--- a/Tones_Task/practice.xlsx
+++ b/Tones_Task/practice.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="15260" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="practice.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t>soundA</t>
   </si>
@@ -49,26 +49,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[u'[1, 3, 5, 6, 8]']</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[u'[1, 3, 5, 6, 9.5]']</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[u'[3, 5, 8, 6, 1]']</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[u'[1.0, 6, 3, 4, 0]']</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[u'[1.0, 6, 4, 3, 0]']</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[u"['C', 4]"]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -93,30 +73,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>['No Scale, 1']</t>
-  </si>
-  <si>
-    <t>['UUUU']</t>
-  </si>
-  <si>
-    <t>['UUDD']</t>
-  </si>
-  <si>
-    <t>['UDUD']</t>
-  </si>
-  <si>
-    <t>['1']</t>
-  </si>
-  <si>
     <t>['0']</t>
   </si>
   <si>
     <t>['2']</t>
   </si>
   <si>
-    <t>['five']</t>
-  </si>
-  <si>
     <t>['none']</t>
   </si>
   <si>
@@ -126,20 +88,86 @@
     <t>['four']</t>
   </si>
   <si>
-    <t>['No Scale, 0.5']</t>
+    <t>[u'[3, 5]']</t>
+  </si>
+  <si>
+    <t>[u'[1.0, 7.0]']</t>
+  </si>
+  <si>
+    <t>[ u'Scale, 2']</t>
+  </si>
+  <si>
+    <t>['U']</t>
+  </si>
+  <si>
+    <t>['one']</t>
+  </si>
+  <si>
+    <t>['two']</t>
+  </si>
+  <si>
+    <t>['']</t>
+  </si>
+  <si>
+    <t>['D']</t>
+  </si>
+  <si>
+    <t>[u'[3.0, 4.0, 10]']</t>
+  </si>
+  <si>
+    <t>[u'Scale, 2']</t>
+  </si>
+  <si>
+    <t>['changes']</t>
+  </si>
+  <si>
+    <t>[u'[5, 6, 10]']</t>
+  </si>
+  <si>
+    <t>[u'Different Scale, 2']</t>
+  </si>
+  <si>
+    <t>['UU']</t>
+  </si>
+  <si>
+    <t>[u'different']</t>
+  </si>
+  <si>
+    <t>[u'[3.0, 1.0, 6]']</t>
+  </si>
+  <si>
+    <t>[u'[11, 8]']</t>
+  </si>
+  <si>
+    <t>[u'[1, 3, 6]']</t>
+  </si>
+  <si>
+    <t>[u'[12, 10, 6]']</t>
+  </si>
+  <si>
+    <t>['DD']</t>
+  </si>
+  <si>
+    <t>[u'same']</t>
+  </si>
+  <si>
+    <t>[u'[11, 8, 5, 4, 1]']</t>
+  </si>
+  <si>
+    <t>[u'[13.0, 8, 3.0, 4, 1]']</t>
+  </si>
+  <si>
+    <t>[u'No Scale, 2']</t>
+  </si>
+  <si>
+    <t>[ u"['G', 3]"]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -177,6 +205,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -499,16 +532,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -534,106 +567,202 @@
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
       </c>
       <c r="J4">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>